<commit_message>
Discrete data. results and cleaning
</commit_message>
<xml_diff>
--- a/Results/_clean_results.xlsx
+++ b/Results/_clean_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s164389\Desktop\Afstuderen\Thesis\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B20137C-00C4-40A2-9617-31209A894635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBD5B6B-F1DA-4E70-87DC-08DD5BC9573D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0%" sheetId="1" r:id="rId1"/>
@@ -19,18 +19,31 @@
     <sheet name="20%" sheetId="4" r:id="rId4"/>
     <sheet name="30%" sheetId="5" r:id="rId5"/>
     <sheet name="Inherent missingness" sheetId="6" r:id="rId6"/>
+    <sheet name="Dataset characteristics" sheetId="7" r:id="rId7"/>
+    <sheet name="Robust instances" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="32">
   <si>
     <t>Dataset</t>
   </si>
@@ -109,12 +122,30 @@
   <si>
     <t>Wisconsin breast cancer</t>
   </si>
+  <si>
+    <t>Instances</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Continuous</t>
+  </si>
+  <si>
+    <t>Discrete</t>
+  </si>
+  <si>
+    <t>Classes</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +157,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,12 +202,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,7 +1010,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="B3:K15"/>
+      <selection sqref="A1:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,7 +1526,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="B3:K15"/>
+      <selection sqref="A1:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1999,8 +2041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E602FCB-125C-44ED-82BD-812C801FC0AB}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="B3:K15"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection sqref="A1:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2516,7 +2558,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:K15"/>
+      <selection sqref="A1:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3032,7 +3074,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="B3:K6"/>
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3226,4 +3268,1060 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A374D30-2240-496E-9BAA-13B1F4434C70}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>625</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>1728</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>1473</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>366</v>
+      </c>
+      <c r="C5">
+        <v>34</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>33</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>13</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>214</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>306</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>155</v>
+      </c>
+      <c r="C9">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>368</v>
+      </c>
+      <c r="C10">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>15</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>435</v>
+      </c>
+      <c r="C11">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>150</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>146</v>
+      </c>
+      <c r="C13">
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>18</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>12960</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>8</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>683</v>
+      </c>
+      <c r="C15">
+        <v>35</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>35</v>
+      </c>
+      <c r="F15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>178</v>
+      </c>
+      <c r="C16">
+        <v>13</v>
+      </c>
+      <c r="D16">
+        <v>13</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>699</v>
+      </c>
+      <c r="C17">
+        <v>9</v>
+      </c>
+      <c r="D17">
+        <v>9</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>101</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>16</v>
+      </c>
+      <c r="F18">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B4B9C2-EE98-45C2-B2BD-185FA7CC9E20}">
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>625</v>
+      </c>
+      <c r="C3" s="5">
+        <v>620.01282252546969</v>
+      </c>
+      <c r="D3" s="5">
+        <v>617.67977301094913</v>
+      </c>
+      <c r="E3" s="5">
+        <v>621.10601557936684</v>
+      </c>
+      <c r="F3" s="5">
+        <v>618.95291850900344</v>
+      </c>
+      <c r="G3" s="5">
+        <v>619.50498554861792</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>1728</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1728</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1728</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1728</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1728</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>1473</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1456.9420923313928</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1460.880947012048</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1458.2752415146531</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1462.8518181863533</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1455.1956319673304</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>366</v>
+      </c>
+      <c r="C6" s="5">
+        <v>141.12329737441195</v>
+      </c>
+      <c r="D6" s="5">
+        <v>136.6645031691279</v>
+      </c>
+      <c r="E6" s="5">
+        <v>128.13261942673344</v>
+      </c>
+      <c r="F6" s="5">
+        <v>130.37735598795643</v>
+      </c>
+      <c r="G6" s="5">
+        <v>121.82851152251381</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>1000</v>
+      </c>
+      <c r="C7" s="5">
+        <v>107.10936287276245</v>
+      </c>
+      <c r="D7" s="5">
+        <v>104.416954963271</v>
+      </c>
+      <c r="E7" s="5">
+        <v>102.21284709033951</v>
+      </c>
+      <c r="F7" s="5">
+        <v>97.017014253152851</v>
+      </c>
+      <c r="G7" s="5">
+        <v>86.616977042520688</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>214</v>
+      </c>
+      <c r="C8" s="5">
+        <v>3.2923076923076913</v>
+      </c>
+      <c r="D8" s="5">
+        <v>3.292307692307693</v>
+      </c>
+      <c r="E8" s="5">
+        <v>3.2923076923076922</v>
+      </c>
+      <c r="F8" s="5">
+        <v>3.292307692307693</v>
+      </c>
+      <c r="G8" s="5">
+        <v>3.2923076923076926</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>306</v>
+      </c>
+      <c r="C9" s="5">
+        <v>275.81936515099812</v>
+      </c>
+      <c r="D9" s="5">
+        <v>278.3044462519793</v>
+      </c>
+      <c r="E9" s="5">
+        <v>278.81746739640124</v>
+      </c>
+      <c r="F9" s="5">
+        <v>271.82476976754191</v>
+      </c>
+      <c r="G9" s="5">
+        <v>272.50304028542331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>150</v>
+      </c>
+      <c r="C10" s="5">
+        <v>96.853963947637894</v>
+      </c>
+      <c r="D10" s="5">
+        <v>94.542295858409602</v>
+      </c>
+      <c r="E10" s="5">
+        <v>91.827279905081667</v>
+      </c>
+      <c r="F10" s="5">
+        <v>88.933124737411418</v>
+      </c>
+      <c r="G10" s="5">
+        <v>81.992478991664925</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>146</v>
+      </c>
+      <c r="C11" s="5">
+        <v>118.66199119630572</v>
+      </c>
+      <c r="D11" s="5">
+        <v>117.48438342027147</v>
+      </c>
+      <c r="E11" s="5">
+        <v>117.07376577203171</v>
+      </c>
+      <c r="F11" s="5">
+        <v>119.42223779866333</v>
+      </c>
+      <c r="G11" s="5">
+        <v>119.94842883863969</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>12960</v>
+      </c>
+      <c r="C12" s="5">
+        <v>10057.790021493982</v>
+      </c>
+      <c r="D12" s="5">
+        <v>10259.668316634046</v>
+      </c>
+      <c r="E12" s="5">
+        <v>10247.461269259567</v>
+      </c>
+      <c r="F12" s="5">
+        <v>10343.147539292966</v>
+      </c>
+      <c r="G12" s="5">
+        <v>10571.770746514285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>178</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>699</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>101</v>
+      </c>
+      <c r="C15" s="5">
+        <v>60.056989247311833</v>
+      </c>
+      <c r="D15" s="5">
+        <v>59.296774193548387</v>
+      </c>
+      <c r="E15" s="5">
+        <v>60.274193548387082</v>
+      </c>
+      <c r="F15" s="5">
+        <v>59.948387096774198</v>
+      </c>
+      <c r="G15" s="5">
+        <v>61.57741935483871</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>625</v>
+      </c>
+      <c r="C19" s="5">
+        <v>625</v>
+      </c>
+      <c r="D19" s="5">
+        <v>619.54503907851142</v>
+      </c>
+      <c r="E19" s="5">
+        <v>616.56371863698735</v>
+      </c>
+      <c r="F19" s="5">
+        <v>608.72826898774179</v>
+      </c>
+      <c r="G19" s="5">
+        <v>597.11997244312931</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>1728</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1728</v>
+      </c>
+      <c r="D20" s="5">
+        <v>1707.9075717219323</v>
+      </c>
+      <c r="E20" s="5">
+        <v>1677.2957499181321</v>
+      </c>
+      <c r="F20" s="5">
+        <v>1410.3855144803506</v>
+      </c>
+      <c r="G20" s="5">
+        <v>1100.8083638806052</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>1473</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1473</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1199.8856822520863</v>
+      </c>
+      <c r="E21" s="5">
+        <v>1029.9035011162027</v>
+      </c>
+      <c r="F21" s="5">
+        <v>678.0588534743182</v>
+      </c>
+      <c r="G21" s="5">
+        <v>732.90252631515216</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22">
+        <v>366</v>
+      </c>
+      <c r="C22" s="5">
+        <v>366</v>
+      </c>
+      <c r="D22" s="5">
+        <v>366</v>
+      </c>
+      <c r="E22" s="5">
+        <v>365.65903004523261</v>
+      </c>
+      <c r="F22" s="5">
+        <v>365.43006078533938</v>
+      </c>
+      <c r="G22" s="5">
+        <v>364.99145069853944</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <v>1000</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1000</v>
+      </c>
+      <c r="D23" s="5">
+        <v>802.57124318543197</v>
+      </c>
+      <c r="E23" s="5">
+        <v>551.03372152226859</v>
+      </c>
+      <c r="F23" s="5">
+        <v>816.25850431022059</v>
+      </c>
+      <c r="G23" s="5">
+        <v>856.25453722885652</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24">
+        <v>214</v>
+      </c>
+      <c r="C24" s="5">
+        <v>214.00000000000003</v>
+      </c>
+      <c r="D24" s="5">
+        <v>212.00029710066156</v>
+      </c>
+      <c r="E24" s="5">
+        <v>210.76188897101525</v>
+      </c>
+      <c r="F24" s="5">
+        <v>205.97112572824761</v>
+      </c>
+      <c r="G24" s="5">
+        <v>208.0393242623513</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25">
+        <v>306</v>
+      </c>
+      <c r="C25" s="5">
+        <v>306</v>
+      </c>
+      <c r="D25" s="5">
+        <v>299.85771576150461</v>
+      </c>
+      <c r="E25" s="5">
+        <v>296.42442661553912</v>
+      </c>
+      <c r="F25" s="5">
+        <v>289.86185930821119</v>
+      </c>
+      <c r="G25" s="5">
+        <v>286.44344976426692</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26">
+        <v>150</v>
+      </c>
+      <c r="C26" s="5">
+        <v>150</v>
+      </c>
+      <c r="D26" s="5">
+        <v>149.54525541049682</v>
+      </c>
+      <c r="E26" s="5">
+        <v>149.67115070943754</v>
+      </c>
+      <c r="F26" s="5">
+        <v>149.88697495925842</v>
+      </c>
+      <c r="G26" s="5">
+        <v>149.67089674056132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>146</v>
+      </c>
+      <c r="C27" s="5">
+        <v>146</v>
+      </c>
+      <c r="D27" s="5">
+        <v>144.34688686245127</v>
+      </c>
+      <c r="E27" s="5">
+        <v>138.38585962778674</v>
+      </c>
+      <c r="F27" s="5">
+        <v>129.84415719798631</v>
+      </c>
+      <c r="G27" s="5">
+        <v>127.96796826180086</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28">
+        <v>12960</v>
+      </c>
+      <c r="C28" s="5">
+        <v>12960</v>
+      </c>
+      <c r="D28" s="5">
+        <v>8296.3937842215928</v>
+      </c>
+      <c r="E28" s="5">
+        <v>7265.6199358458343</v>
+      </c>
+      <c r="F28" s="5">
+        <v>6424.0804106857449</v>
+      </c>
+      <c r="G28" s="5">
+        <v>6039.2378661764797</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29">
+        <v>178</v>
+      </c>
+      <c r="C29" s="5">
+        <v>178</v>
+      </c>
+      <c r="D29" s="5">
+        <v>177.89391627729569</v>
+      </c>
+      <c r="E29" s="5">
+        <v>178</v>
+      </c>
+      <c r="F29" s="5">
+        <v>177.45533469329663</v>
+      </c>
+      <c r="G29" s="5">
+        <v>177.55820965952464</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <v>699</v>
+      </c>
+      <c r="C30" s="5">
+        <v>699</v>
+      </c>
+      <c r="D30" s="5">
+        <v>698.8659835359889</v>
+      </c>
+      <c r="E30" s="5">
+        <v>698.73042412762902</v>
+      </c>
+      <c r="F30" s="5">
+        <v>698.72166565287171</v>
+      </c>
+      <c r="G30" s="5">
+        <v>698.86251269026218</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>101</v>
+      </c>
+      <c r="C31" s="5">
+        <v>101</v>
+      </c>
+      <c r="D31" s="5">
+        <v>100.77062242580546</v>
+      </c>
+      <c r="E31" s="5">
+        <v>100.77220077220076</v>
+      </c>
+      <c r="F31" s="5">
+        <v>100.66561441330458</v>
+      </c>
+      <c r="G31" s="5">
+        <v>100.67649442364835</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>